<commit_message>
update saved and temp model.. save model in prev commit, sl:3121 s:5T temp:50_50T 7/4/2025
</commit_message>
<xml_diff>
--- a/temp_models/accuracies/max_r_model_accuracies.xlsx
+++ b/temp_models/accuracies/max_r_model_accuracies.xlsx
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0.9613333333333334</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6</v>
+        <v>0.7873333333333333</v>
       </c>
     </row>
     <row r="3">
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0.9593333333333334</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6</v>
+        <v>0.8113333333333334</v>
       </c>
     </row>
     <row r="4">
@@ -483,10 +483,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0.956</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6</v>
+        <v>0.7646666666666667</v>
       </c>
     </row>
     <row r="5">
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0.9633333333333334</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6</v>
+        <v>0.802</v>
       </c>
     </row>
     <row r="6">
@@ -509,10 +509,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>0.9613333333333334</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6</v>
+        <v>0.7733333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change temp model sl:3121 90/10 random 7/4/2025
</commit_message>
<xml_diff>
--- a/temp_models/accuracies/max_r_model_accuracies.xlsx
+++ b/temp_models/accuracies/max_r_model_accuracies.xlsx
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9613333333333334</v>
+        <v>0.9552715654952076</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7873333333333333</v>
+        <v>0.8115015974440895</v>
       </c>
     </row>
     <row r="3">
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9593333333333334</v>
+        <v>0.9680511182108626</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8113333333333334</v>
+        <v>0.8402555910543131</v>
       </c>
     </row>
     <row r="4">
@@ -483,10 +483,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.956</v>
+        <v>0.9744408945686901</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7646666666666667</v>
+        <v>0.7731629392971247</v>
       </c>
     </row>
     <row r="5">
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9633333333333334</v>
+        <v>0.9744408945686901</v>
       </c>
       <c r="C5" t="n">
-        <v>0.802</v>
+        <v>0.8338658146964856</v>
       </c>
     </row>
     <row r="6">
@@ -509,10 +509,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9613333333333334</v>
+        <v>0.9680511182108626</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7733333333333333</v>
+        <v>0.8274760383386581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>